<commit_message>
udpated tutoring to remove darren
</commit_message>
<xml_diff>
--- a/CS320-Sp18-TutoringSchedule.xlsx
+++ b/CS320-Sp18-TutoringSchedule.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\djhake2\cs320-spring2018\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="150" yWindow="90" windowWidth="26535" windowHeight="11655"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="20">
   <si>
     <t>Monday (in class)</t>
   </si>
@@ -63,13 +68,7 @@
     <t>Cody Spath</t>
   </si>
   <si>
-    <t>Darren Webb</t>
-  </si>
-  <si>
     <t>Corey Wolf</t>
-  </si>
-  <si>
-    <t>CS320: Software Engineering Tutoring Schedule (tentative)</t>
   </si>
   <si>
     <t>Evenings
@@ -80,6 +79,9 @@
   </si>
   <si>
     <t>Evening Schedule</t>
+  </si>
+  <si>
+    <t>CS320: Software Engineering Tutoring Schedule (tentative - starts Weds, 1-24-18)</t>
   </si>
 </sst>
 </file>
@@ -361,40 +363,40 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -405,6 +407,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -453,7 +458,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -488,7 +493,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -697,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:Y24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -750,34 +755,34 @@
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
     </row>
-    <row r="2" spans="1:25" s="29" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="28"/>
-      <c r="W2" s="28"/>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="28"/>
+    <row r="2" spans="1:25" s="24" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
     </row>
     <row r="3" spans="1:25" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -807,26 +812,26 @@
       <c r="Y3" s="3"/>
     </row>
     <row r="4" spans="1:25" s="4" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="24" t="s">
+      <c r="A4" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="20"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="32"/>
       <c r="I4" s="6"/>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="19"/>
-      <c r="L4" s="20"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="32"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
@@ -837,36 +842,36 @@
       <c r="T4" s="3"/>
     </row>
     <row r="5" spans="1:25" s="4" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="25">
         <v>0.375</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="25">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="25">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="31">
+      <c r="F5" s="25">
         <v>0.375</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="25">
         <v>0.45833333333333331</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="25">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I5" s="6"/>
-      <c r="J5" s="31">
+      <c r="J5" s="25">
         <v>0.375</v>
       </c>
-      <c r="K5" s="31">
+      <c r="K5" s="25">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L5" s="31">
+      <c r="L5" s="25">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
@@ -966,7 +971,7 @@
     </row>
     <row r="10" spans="1:25" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="16" t="s">
@@ -989,15 +994,15 @@
     <row r="11" spans="1:25" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:25" s="4" customFormat="1" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="32" t="s">
+      <c r="A13" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
+      <c r="B13" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
       <c r="F13" s="2"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1009,19 +1014,19 @@
       <c r="N13" s="3"/>
     </row>
     <row r="14" spans="1:25" s="4" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F14" s="2"/>
@@ -1103,34 +1108,33 @@
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+    </row>
     <row r="24" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1143,19 +1147,6 @@
       <c r="L24" s="5"/>
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
-    </row>
-    <row r="25" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>